<commit_message>
2024-03-01 Friday, 13:35Auto Push
</commit_message>
<xml_diff>
--- a/2024-03-01 Friday.xlsx
+++ b/2024-03-01 Friday.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,58 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>206</v>
+      </c>
+      <c r="B2" t="n">
+        <v>14</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>許*綸</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-03-01 12:59:50</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>206</v>
+      </c>
+      <c r="B3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>許*綸</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2024-03-01 12:59:39</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-03-01 12:59:47</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>OUT</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>